<commit_message>
fix: excel for overtime
</commit_message>
<xml_diff>
--- a/public/overtime_file/overtime-template.xlsx
+++ b/public/overtime_file/overtime-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedric\Desktop\laravel-hris\public\overtime_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2E7FAD-486F-4A73-9252-1072E062E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D97986-F72A-4604-A7CB-0D42D20232F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A99CA247-AE5D-4DD5-A5F5-529A717BE116}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>EMPLOYEE_NO</t>
   </si>
   <si>
-    <t>ATTENDANCE_DATE</t>
+    <t>OVERTIME_DATE</t>
   </si>
   <si>
-    <t>ATTENDANCE_TIME</t>
+    <t>OVERTIME_IN</t>
   </si>
   <si>
-    <t>ATTENDANCE_OUT</t>
+    <t>OVERTIME_OUT</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>